<commit_message>
modificaciones en tabla de riesgos
modificaciones en tabla de riesgos
</commit_message>
<xml_diff>
--- a/Docs/Entrega3/tablas.xlsx
+++ b/Docs/Entrega3/tablas.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AdquisicionRecursos" sheetId="1" r:id="rId1"/>
     <sheet name="Entrenamiento" sheetId="2" r:id="rId2"/>
     <sheet name="PlanDePersonal" sheetId="4" r:id="rId3"/>
     <sheet name="asignacionEsfuerzo" sheetId="3" r:id="rId4"/>
+    <sheet name="riesgos" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="108">
   <si>
     <t>Recurso</t>
   </si>
@@ -249,15 +250,120 @@
   <si>
     <t>Tester</t>
   </si>
+  <si>
+    <t>Id Riesgo</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Probabilidad</t>
+  </si>
+  <si>
+    <t>Impacto</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incendio  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terremoto </t>
+  </si>
+  <si>
+    <t>Corte del suministro eléctrico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paro del personal  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No se cumple con la calidad  </t>
+  </si>
+  <si>
+    <t>Problemas financieros fuerzan a reducir el presupuesto</t>
+  </si>
+  <si>
+    <t>No se cumple con la fecha de entrega</t>
+  </si>
+  <si>
+    <t>Los requerimientos cambian rápidamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal clave enfermo o no disponible en momentos críticos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se gasta más del presupuesto  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta el financiamiento previsto en el plan  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta liderazgo para coordinar equipos  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambian las normativas legales  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La agenda inicial es irreal  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta capacitación del personal  </t>
+  </si>
+  <si>
+    <t>La capacitación necesaria para el personal no está disponible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falla la comunicación entre el equipo de trabajo  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controles de calidad inadecuados  </t>
+  </si>
+  <si>
+    <t>Falta soporte técnico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requisitos mal interpretados </t>
+  </si>
+  <si>
+    <t>Retraso en la entrega de los servidores por parte del proveedor de hardware</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>alto</t>
+  </si>
+  <si>
+    <t>baja</t>
+  </si>
+  <si>
+    <t>alta</t>
+  </si>
+  <si>
+    <t>medio</t>
+  </si>
+  <si>
+    <t>F. Guillemet</t>
+  </si>
+  <si>
+    <t>G. Picci</t>
+  </si>
+  <si>
+    <t>L. Svetlich</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,16 +384,29 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAEAEA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -336,11 +455,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -348,12 +482,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -371,6 +505,12 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,7 +1113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
@@ -1573,4 +1713,402 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>